<commit_message>
se agregan loc a programa 'bookshelf' SQLite
</commit_message>
<xml_diff>
--- a/SQLite Programs/bookstore-sqlite/bookstore.xlsx
+++ b/SQLite Programs/bookstore-sqlite/bookstore.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -27,32 +27,16 @@
     <t>Author</t>
   </si>
   <si>
-    <t>emilia</t>
-  </si>
-  <si>
-    <t>cinco</t>
-  </si>
-  <si>
-    <t>
-</t>
-  </si>
-  <si>
-    <t>cinco pepitas de naranja</t>
-  </si>
-  <si>
-    <t>the united states in literature</t>
-  </si>
-  <si>
-    <t>el</t>
-  </si>
-  <si>
-    <t>a love supreme</t>
-  </si>
-  <si>
-    <t>john coltrane</t>
-  </si>
-  <si>
-    <t>blue trane</t>
+    <t>A Love Supreme</t>
+  </si>
+  <si>
+    <t>John Coltrane</t>
+  </si>
+  <si>
+    <t>VALIS</t>
+  </si>
+  <si>
+    <t>Philip K. Dick</t>
   </si>
 </sst>
 </file>
@@ -419,7 +403,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -447,101 +431,22 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s"/>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s"/>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s"/>
-      <c r="C6" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s"/>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s"/>
-      <c r="C8" s="1" t="s"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s"/>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s"/>
-      <c r="C10" s="1" t="s"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>